<commit_message>
OK, creo que ahora si tengo todo, deperar un poco los errores para que saque mejor lo que quiero (los controlados bien), pero Ok
</commit_message>
<xml_diff>
--- a/app/datos/cierre_caja/resultado_openpyxl.xlsx
+++ b/app/datos/cierre_caja/resultado_openpyxl.xlsx
@@ -1,7 +1,25 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="LOCAL LM" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
+</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -31,8 +49,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -390,4 +411,476 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tienda</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Nombre_TPV</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>fecha</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>cierre_tpv_desc</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Nombre_MdP</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>total_ventas</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>total_operaciones</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>GLOVO</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>190.6</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SMS</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>1915.04</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>4663.5</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>295.5</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>857.99</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>563.28</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>GLOVO</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>73.8</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="n">
+        <v>1351.34</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>2196.68</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>1107.08</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>563.28</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>GLOVO</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>73.8</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Tarde</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>1351.34</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>EUROS</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>295.5</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>LOCAL LM</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>45570</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Mañana</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>TARJETA VISA</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>857.99</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>